<commit_message>
upgrade to tiefaces 1.0.0
</commit_message>
<xml_diff>
--- a/src/main/resources/websheet/PRICELIST.xlsx
+++ b/src/main/resources/websheet/PRICELIST.xlsx
@@ -1,31 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28692" windowHeight="13056" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Sale Price Report" sheetId="1" r:id="rId1"/>
-    <sheet name="Configuration" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sale Price Report'!$A$1:$D$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sale Price Report'!$A$1:$D$7</definedName>
     <definedName name="solver_eng" localSheetId="0">1</definedName>
     <definedName name="solver_neg" localSheetId="0">1</definedName>
     <definedName name="solver_num" localSheetId="0">0</definedName>
-    <definedName name="solver_opt" localSheetId="0">'Sale Price Report'!$B$4</definedName>
+    <definedName name="solver_opt" localSheetId="0">'Sale Price Report'!$B$3</definedName>
     <definedName name="solver_typ" localSheetId="0">1</definedName>
     <definedName name="solver_val" localSheetId="0">0</definedName>
     <definedName name="solver_ver" localSheetId="0">3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Jason</author>
+    <author>Jiang, Jason (MOHLTC)</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+          </rPr>
+          <t xml:space="preserve">tie:form(name="sale report" length="7" headerLength="4" footerLength="1")
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>tie:each(items="items", var="item", length="1")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Sale Price Report</t>
   </si>
@@ -55,6 +91,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">  If you require help, please email to: </t>
     </r>
     <r>
@@ -63,152 +105,88 @@
         <sz val="10"/>
         <color indexed="48"/>
         <rFont val="Arial"/>
-        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>Jason.Jiang.ca@gmail.com</t>
     </r>
   </si>
   <si>
-    <t>Tab Name</t>
-  </si>
-  <si>
-    <t>Sheet Name</t>
-  </si>
-  <si>
-    <t>Form Header Range</t>
-  </si>
-  <si>
-    <t>Form Body Range</t>
-  </si>
-  <si>
-    <t>Form Footer Range</t>
-  </si>
-  <si>
-    <t>Form Body Type</t>
-  </si>
-  <si>
-    <t>Allow ADD/DELETE ROW</t>
-  </si>
-  <si>
-    <t>Initial Rows</t>
-  </si>
-  <si>
-    <t>Form Page Type</t>
-  </si>
-  <si>
-    <t>Target Column/Cell</t>
-  </si>
-  <si>
-    <t>Attributes Type</t>
-  </si>
-  <si>
-    <t>Attributes Value</t>
-  </si>
-  <si>
-    <t>Validation Error Messages</t>
-  </si>
-  <si>
-    <t>$A$3 : $D$5</t>
-  </si>
-  <si>
-    <t>$A$6 : $D$8</t>
-  </si>
-  <si>
-    <t>Repeat</t>
-  </si>
-  <si>
-    <t>#{webSheetReports_Data.rowCount}</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>$A</t>
-  </si>
-  <si>
-    <t>Load</t>
-  </si>
-  <si>
-    <t>#{webSheetReports_Data.itemList[$rowIndex].code}</t>
-  </si>
-  <si>
-    <t>$B</t>
-  </si>
-  <si>
-    <t>#{webSheetReports_Data.itemList[$rowIndex].name}</t>
-  </si>
-  <si>
-    <t>$C</t>
-  </si>
-  <si>
-    <t>#{webSheetReports_Data.itemList[$rowIndex].description}</t>
-  </si>
-  <si>
-    <t>$D</t>
-  </si>
-  <si>
-    <t>#{webSheetReports_Data.itemList[$rowIndex].price}</t>
+    <t>${item.name}</t>
+  </si>
+  <si>
+    <t>${item.description}</t>
+  </si>
+  <si>
+    <t>${item.price}</t>
+  </si>
+  <si>
+    <t>${item.code}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="20"/>
-      <color indexed="18"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="8"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color indexed="48"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,12 +201,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="27"/>
         <bgColor indexed="41"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -244,6 +234,19 @@
         <color indexed="8"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -297,77 +300,67 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -672,29 +665,17 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
           <a:headEnd type="none" w="med" len="med"/>
           <a:tailEnd type="none" w="med" len="med"/>
         </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
       </a:spPr>
       <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
       <a:lstStyle/>
@@ -714,29 +695,17 @@
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
           <a:headEnd type="none" w="med" len="med"/>
           <a:tailEnd type="none" w="med" len="med"/>
         </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
       </a:spPr>
       <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
       <a:lstStyle/>
@@ -747,245 +716,106 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:D7"/>
+    <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.1640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.33203125" style="1"/>
+    <col min="1" max="1" width="20.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="29.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.109375" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.33203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:4" ht="33" customHeight="1">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
-    <row r="2" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="D2" s="2"/>
+    <row r="2" spans="1:4" ht="24" customHeight="1">
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
-    <row r="3" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+    <row r="3" spans="1:4" ht="35.4" customHeight="1">
+      <c r="A3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>3</v>
-      </c>
+    <row r="4" spans="1:4" ht="22.2" customHeight="1">
+      <c r="A4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
+    <row r="5" spans="1:4" s="1" customFormat="1" ht="24.6" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="C5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="11" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="10"/>
+    <row r="6" spans="1:4" ht="28.95" customHeight="1">
+      <c r="A6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
     </row>
-    <row r="7" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-    </row>
-    <row r="8" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+    <row r="7" spans="1:4" ht="21.6" customHeight="1">
+      <c r="A7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="6">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
   </mergeCells>
-  <pageMargins left="0.69930555555555551" right="0.69930555555555551" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup scale="55" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.69791666666666696" right="0.69791666666666696" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
+  <pageSetup scale="55" firstPageNumber="0" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="16.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="29" style="13" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="33.83203125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="13" customWidth="1"/>
-    <col min="12" max="12" width="43.6640625" style="13" customWidth="1"/>
-    <col min="13" max="13" width="57.1640625" style="13" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="13" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="14"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J3" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="14"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J4" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="14"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J5" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="14"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <pageMargins left="0.69930555555555551" right="0.69930555555555551" top="0.75" bottom="0.75" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change description and home page.
</commit_message>
<xml_diff>
--- a/src/main/resources/websheet/PRICELIST.xlsx
+++ b/src/main/resources/websheet/PRICELIST.xlsx
@@ -37,7 +37,7 @@
             <sz val="9"/>
             <rFont val="Times New Roman"/>
           </rPr>
-          <t xml:space="preserve">tie:form(name="sale report" length="7" headerLength="4" footerLength="1")
+          <t xml:space="preserve">tie:form(name="sale report" length="7" headerLength="4" footerLength="0")
 </t>
         </r>
       </text>
@@ -720,7 +720,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2"/>

</xml_diff>